<commit_message>
deep refactoring according to OOP guidelines
</commit_message>
<xml_diff>
--- a/vocabulary.xlsx
+++ b/vocabulary.xlsx
@@ -12480,7 +12480,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="11" s="17" spans="1:12">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="28" t="s">
         <v>42</v>
       </c>
       <c r="C11" s="25" t="s">
@@ -12634,7 +12634,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="17" s="17" spans="1:12">
-      <c r="A17" s="24" t="s">
+      <c r="A17" s="28" t="s">
         <v>75</v>
       </c>
       <c r="C17" s="25" t="s">
@@ -12659,7 +12659,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="18" s="17" spans="1:12">
-      <c r="A18" s="24" t="s">
+      <c r="A18" s="28" t="s">
         <v>80</v>
       </c>
       <c r="C18" s="22" t="n"/>
@@ -12724,7 +12724,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="21" s="17" spans="1:12">
-      <c r="A21" s="21" t="s">
+      <c r="A21" s="28" t="s">
         <v>89</v>
       </c>
       <c r="C21" s="25" t="s">
@@ -12797,7 +12797,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="24" s="17" spans="1:12">
-      <c r="A24" s="24" t="s">
+      <c r="A24" s="30" t="s">
         <v>103</v>
       </c>
       <c r="C24" s="25" t="s">
@@ -12893,7 +12893,7 @@
       </c>
     </row>
     <row customHeight="1" ht="12.95" r="28" s="17" spans="1:12">
-      <c r="A28" s="21" t="s">
+      <c r="A28" s="30" t="s">
         <v>119</v>
       </c>
       <c r="C28" s="25" t="s">
@@ -12918,7 +12918,7 @@
       </c>
     </row>
     <row customHeight="1" ht="35.95" r="29" s="17" spans="1:12">
-      <c r="A29" s="21" t="s">
+      <c r="A29" s="28" t="s">
         <v>124</v>
       </c>
       <c r="C29" s="25" t="s">
@@ -12974,7 +12974,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="31" s="17" spans="1:12">
-      <c r="A31" s="21" t="s">
+      <c r="A31" s="28" t="s">
         <v>137</v>
       </c>
       <c r="C31" s="25" t="s">
@@ -13147,7 +13147,7 @@
       </c>
     </row>
     <row customHeight="1" ht="35.95" r="38" s="17" spans="1:12">
-      <c r="A38" s="21" t="s">
+      <c r="A38" s="28" t="s">
         <v>172</v>
       </c>
       <c r="C38" s="25" t="s">
@@ -13241,7 +13241,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="42" s="17" spans="1:12">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="28" t="s">
         <v>189</v>
       </c>
       <c r="C42" s="22" t="n"/>
@@ -13283,7 +13283,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="44" s="17" spans="1:12">
-      <c r="A44" s="21" t="s">
+      <c r="A44" s="28" t="s">
         <v>195</v>
       </c>
       <c r="C44" s="25" t="s">
@@ -13348,7 +13348,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="47" s="17" spans="1:12">
-      <c r="A47" s="21" t="s">
+      <c r="A47" s="30" t="s">
         <v>204</v>
       </c>
       <c r="C47" s="22" t="n"/>
@@ -13417,7 +13417,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="50" s="17" spans="1:12">
-      <c r="A50" s="24" t="s">
+      <c r="A50" s="28" t="s">
         <v>217</v>
       </c>
       <c r="C50" s="25" t="s">
@@ -13559,7 +13559,7 @@
       </c>
     </row>
     <row customHeight="1" ht="12.95" r="56" s="17" spans="1:12">
-      <c r="A56" s="21" t="s">
+      <c r="A56" s="30" t="s">
         <v>243</v>
       </c>
       <c r="C56" s="25" t="s">
@@ -13584,7 +13584,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="57" s="17" spans="1:12">
-      <c r="A57" s="21" t="s">
+      <c r="A57" s="28" t="s">
         <v>249</v>
       </c>
       <c r="C57" s="25" t="s">
@@ -13705,7 +13705,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="62" s="17" spans="1:12">
-      <c r="A62" s="24" t="s">
+      <c r="A62" s="28" t="s">
         <v>272</v>
       </c>
       <c r="C62" s="25" t="s">
@@ -13926,7 +13926,7 @@
       </c>
     </row>
     <row customHeight="1" ht="17.95" r="71" s="17" spans="1:12">
-      <c r="A71" s="21" t="s">
+      <c r="A71" s="28" t="s">
         <v>313</v>
       </c>
       <c r="C71" s="22" t="n"/>
@@ -14089,7 +14089,7 @@
       </c>
     </row>
     <row customHeight="1" ht="17.95" r="78" s="17" spans="1:12">
-      <c r="A78" s="21" t="s">
+      <c r="A78" s="28" t="s">
         <v>345</v>
       </c>
       <c r="C78" s="22" t="n"/>
@@ -14131,7 +14131,7 @@
       </c>
     </row>
     <row customHeight="1" ht="12.95" r="80" s="17" spans="1:12">
-      <c r="A80" s="21" t="s">
+      <c r="A80" s="30" t="s">
         <v>353</v>
       </c>
       <c r="C80" s="25" t="s">
@@ -14183,7 +14183,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="82" s="17" spans="1:12">
-      <c r="A82" s="21" t="s">
+      <c r="A82" s="28" t="s">
         <v>366</v>
       </c>
       <c r="C82" s="27" t="s">
@@ -14336,7 +14336,7 @@
       </c>
     </row>
     <row customHeight="1" ht="35.95" r="89" s="17" spans="1:12">
-      <c r="A89" s="21" t="s">
+      <c r="A89" s="28" t="s">
         <v>397</v>
       </c>
       <c r="C89" s="25" t="s">
@@ -14374,7 +14374,7 @@
       </c>
     </row>
     <row customHeight="1" ht="35.95" r="91" s="17" spans="1:12">
-      <c r="A91" s="21" t="s">
+      <c r="A91" s="28" t="s">
         <v>403</v>
       </c>
       <c r="C91" s="25" t="s">
@@ -14494,7 +14494,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="97" s="17" spans="1:12">
-      <c r="A97" s="21" t="s">
+      <c r="A97" s="28" t="s">
         <v>424</v>
       </c>
       <c r="C97" s="22" t="n"/>
@@ -14513,7 +14513,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="98" s="17" spans="1:12">
-      <c r="A98" s="21" t="s">
+      <c r="A98" s="26" t="s">
         <v>427</v>
       </c>
       <c r="C98" s="22" t="n"/>
@@ -14574,7 +14574,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="101" s="17" spans="1:12">
-      <c r="A101" s="21" t="s">
+      <c r="A101" s="28" t="s">
         <v>438</v>
       </c>
       <c r="C101" s="22" t="n"/>
@@ -14692,7 +14692,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="107" s="17" spans="1:12">
-      <c r="A107" s="21" t="s">
+      <c r="A107" s="26" t="s">
         <v>458</v>
       </c>
       <c r="C107" s="25" t="s">
@@ -14721,7 +14721,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="108" s="17" spans="1:12">
-      <c r="A108" s="21" t="s">
+      <c r="A108" s="30" t="s">
         <v>466</v>
       </c>
       <c r="C108" s="25" t="s">
@@ -14788,7 +14788,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="111" s="17" spans="1:12">
-      <c r="A111" s="21" t="s">
+      <c r="A111" s="30" t="s">
         <v>480</v>
       </c>
       <c r="C111" s="25" t="s">
@@ -14857,7 +14857,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="114" s="17" spans="1:12">
-      <c r="A114" s="21" t="s">
+      <c r="A114" s="30" t="s">
         <v>494</v>
       </c>
       <c r="C114" s="25" t="s">
@@ -14970,7 +14970,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="119" s="17" spans="1:12">
-      <c r="A119" s="21" t="s">
+      <c r="A119" s="28" t="s">
         <v>517</v>
       </c>
       <c r="C119" s="25" t="s">
@@ -15016,7 +15016,7 @@
       </c>
     </row>
     <row customHeight="1" ht="34.95" r="121" s="17" spans="1:12">
-      <c r="A121" s="21" t="s">
+      <c r="A121" s="28" t="s">
         <v>527</v>
       </c>
       <c r="C121" s="25" t="s">
@@ -15098,7 +15098,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="125" s="17" spans="1:12">
-      <c r="A125" s="21" t="s">
+      <c r="A125" s="26" t="s">
         <v>542</v>
       </c>
       <c r="C125" s="25" t="s">
@@ -15203,7 +15203,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="130" s="17" spans="1:12">
-      <c r="A130" s="21" t="s">
+      <c r="A130" s="28" t="s">
         <v>560</v>
       </c>
       <c r="C130" s="22" t="n"/>
@@ -15249,7 +15249,7 @@
       </c>
     </row>
     <row customHeight="1" ht="12.95" r="132" s="17" spans="1:12">
-      <c r="A132" s="21" t="s">
+      <c r="A132" s="26" t="s">
         <v>570</v>
       </c>
       <c r="C132" s="25" t="s">
@@ -15335,7 +15335,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="136" s="17" spans="1:12">
-      <c r="A136" s="21" t="s">
+      <c r="A136" s="28" t="s">
         <v>586</v>
       </c>
       <c r="C136" s="22" t="n"/>
@@ -15448,7 +15448,7 @@
       </c>
     </row>
     <row customHeight="1" ht="35.95" r="141" s="17" spans="1:12">
-      <c r="A141" s="21" t="s">
+      <c r="A141" s="28" t="s">
         <v>610</v>
       </c>
       <c r="C141" s="22" t="n"/>
@@ -15490,7 +15490,7 @@
       </c>
     </row>
     <row customHeight="1" ht="17.95" r="143" s="17" spans="1:12">
-      <c r="A143" s="21" t="s">
+      <c r="A143" s="28" t="s">
         <v>618</v>
       </c>
       <c r="C143" s="25" t="s">
@@ -15584,7 +15584,7 @@
       </c>
     </row>
     <row customHeight="1" ht="12.95" r="147" s="17" spans="1:12">
-      <c r="A147" s="21" t="s">
+      <c r="A147" s="28" t="s">
         <v>638</v>
       </c>
       <c r="C147" s="25" t="s">
@@ -15645,7 +15645,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="150" s="17" spans="1:12">
-      <c r="A150" s="21" t="s">
+      <c r="A150" s="30" t="s">
         <v>648</v>
       </c>
       <c r="C150" s="25" t="s">
@@ -15695,7 +15695,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="152" s="17" spans="1:12">
-      <c r="A152" s="21" t="s">
+      <c r="A152" s="28" t="s">
         <v>659</v>
       </c>
       <c r="C152" s="25" t="s">
@@ -15741,7 +15741,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="154" s="17" spans="1:12">
-      <c r="A154" s="21" t="s">
+      <c r="A154" s="28" t="s">
         <v>668</v>
       </c>
       <c r="C154" s="22" t="n"/>
@@ -15802,7 +15802,7 @@
       </c>
     </row>
     <row customHeight="1" ht="23.95" r="157" s="17" spans="1:12">
-      <c r="A157" s="21" t="s">
+      <c r="A157" s="26" t="s">
         <v>679</v>
       </c>
       <c r="C157" s="22" t="n"/>
@@ -15823,7 +15823,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="158" s="17" spans="1:12">
-      <c r="A158" s="21" t="s">
+      <c r="A158" s="30" t="s">
         <v>683</v>
       </c>
       <c r="C158" s="25" t="s">
@@ -15842,7 +15842,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="159" s="17" spans="1:12">
-      <c r="A159" s="21" t="s">
+      <c r="A159" s="30" t="s">
         <v>686</v>
       </c>
       <c r="C159" s="22" t="n"/>
@@ -15861,7 +15861,7 @@
       </c>
     </row>
     <row customHeight="1" ht="35.95" r="160" s="17" spans="1:12">
-      <c r="A160" s="21" t="s">
+      <c r="A160" s="30" t="s">
         <v>689</v>
       </c>
       <c r="C160" s="25" t="s">
@@ -15907,7 +15907,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="162" s="17" spans="1:12">
-      <c r="A162" s="21" t="s">
+      <c r="A162" s="26" t="s">
         <v>699</v>
       </c>
       <c r="C162" s="25" t="s">
@@ -15928,7 +15928,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="163" s="17" spans="1:12">
-      <c r="A163" s="21" t="s">
+      <c r="A163" s="26" t="s">
         <v>703</v>
       </c>
       <c r="C163" s="25" t="s">
@@ -15991,7 +15991,7 @@
       </c>
     </row>
     <row customHeight="1" ht="35.95" r="166" s="17" spans="1:12">
-      <c r="A166" s="21" t="s">
+      <c r="A166" s="30" t="s">
         <v>714</v>
       </c>
       <c r="C166" s="22" t="n"/>
@@ -16316,7 +16316,7 @@
       </c>
     </row>
     <row customHeight="1" ht="35.95" r="181" s="17" spans="1:12">
-      <c r="A181" s="21" t="s">
+      <c r="A181" s="30" t="s">
         <v>777</v>
       </c>
       <c r="C181" s="25" t="n"/>
@@ -16381,7 +16381,7 @@
       </c>
     </row>
     <row customHeight="1" ht="23.95" r="184" s="17" spans="1:12">
-      <c r="A184" s="21" t="s">
+      <c r="A184" s="30" t="s">
         <v>789</v>
       </c>
       <c r="C184" s="25" t="s">
@@ -16400,7 +16400,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="185" s="17" spans="1:12">
-      <c r="A185" s="21" t="s">
+      <c r="A185" s="30" t="s">
         <v>792</v>
       </c>
       <c r="C185" s="25" t="s">
@@ -16440,7 +16440,7 @@
       </c>
     </row>
     <row customHeight="1" ht="35.95" r="187" s="17" spans="1:12">
-      <c r="A187" s="21" t="s">
+      <c r="A187" s="26" t="s">
         <v>799</v>
       </c>
       <c r="C187" s="25" t="n"/>
@@ -16459,7 +16459,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="188" s="17" spans="1:12">
-      <c r="A188" s="21" t="s">
+      <c r="A188" s="26" t="s">
         <v>802</v>
       </c>
       <c r="C188" s="25" t="n"/>
@@ -16501,7 +16501,7 @@
       </c>
     </row>
     <row customHeight="1" ht="35.95" r="190" s="17" spans="1:12">
-      <c r="A190" s="21" t="s">
+      <c r="A190" s="26" t="s">
         <v>810</v>
       </c>
       <c r="C190" s="25" t="s">
@@ -16587,7 +16587,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="194" s="17" spans="1:12">
-      <c r="A194" s="30" t="s">
+      <c r="A194" s="28" t="s">
         <v>827</v>
       </c>
       <c r="C194" s="25" t="s">
@@ -16614,7 +16614,7 @@
       </c>
     </row>
     <row customHeight="1" ht="12.95" r="195" s="17" spans="1:12">
-      <c r="A195" s="21" t="s">
+      <c r="A195" s="30" t="s">
         <v>833</v>
       </c>
       <c r="C195" s="25" t="s">
@@ -16654,7 +16654,7 @@
       </c>
     </row>
     <row customHeight="1" ht="35.95" r="197" s="17" spans="1:12">
-      <c r="A197" s="21" t="s">
+      <c r="A197" s="28" t="s">
         <v>840</v>
       </c>
       <c r="C197" s="25" t="n"/>
@@ -16673,7 +16673,7 @@
       </c>
     </row>
     <row customHeight="1" ht="12.95" r="198" s="17" spans="1:12">
-      <c r="A198" s="21" t="s">
+      <c r="A198" s="28" t="s">
         <v>843</v>
       </c>
       <c r="C198" s="25" t="s">
@@ -16740,7 +16740,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="201" s="17" spans="1:12">
-      <c r="A201" s="21" t="s">
+      <c r="A201" s="28" t="s">
         <v>857</v>
       </c>
       <c r="C201" s="25" t="s">
@@ -16761,7 +16761,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="202" s="17" spans="1:12">
-      <c r="A202" s="26" t="s">
+      <c r="A202" s="30" t="s">
         <v>861</v>
       </c>
       <c r="C202" s="25" t="n"/>
@@ -16826,7 +16826,7 @@
       </c>
     </row>
     <row customHeight="1" ht="17.95" r="205" s="17" spans="1:12">
-      <c r="A205" s="21" t="s">
+      <c r="A205" s="26" t="s">
         <v>871</v>
       </c>
       <c r="C205" s="25" t="n"/>
@@ -16849,7 +16849,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="206" s="17" spans="1:12">
-      <c r="A206" s="21" t="s">
+      <c r="A206" s="28" t="s">
         <v>876</v>
       </c>
       <c r="C206" s="25" t="s">
@@ -16872,7 +16872,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="207" s="17" spans="1:12">
-      <c r="A207" s="21" t="s">
+      <c r="A207" s="26" t="s">
         <v>881</v>
       </c>
       <c r="C207" s="25" t="s">
@@ -16893,7 +16893,7 @@
       </c>
     </row>
     <row customHeight="1" ht="35.95" r="208" s="17" spans="1:12">
-      <c r="A208" s="21" t="s">
+      <c r="A208" s="30" t="s">
         <v>885</v>
       </c>
       <c r="C208" s="25" t="s">
@@ -16912,7 +16912,7 @@
       </c>
     </row>
     <row customHeight="1" ht="35.95" r="209" s="17" spans="1:12">
-      <c r="A209" s="21" t="s">
+      <c r="A209" s="30" t="s">
         <v>888</v>
       </c>
       <c r="C209" s="25" t="n"/>
@@ -16992,7 +16992,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="213" s="17" spans="1:12">
-      <c r="A213" s="21" t="s">
+      <c r="A213" s="30" t="s">
         <v>899</v>
       </c>
       <c r="C213" s="25" t="n"/>
@@ -17034,7 +17034,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="215" s="17" spans="1:12">
-      <c r="A215" s="21" t="s">
+      <c r="A215" s="30" t="s">
         <v>907</v>
       </c>
       <c r="C215" s="25" t="s">
@@ -17099,7 +17099,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="218" s="17" spans="1:12">
-      <c r="A218" s="21" t="s">
+      <c r="A218" s="28" t="s">
         <v>920</v>
       </c>
       <c r="C218" s="25" t="s">
@@ -17143,7 +17143,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="220" s="17" spans="1:12">
-      <c r="A220" s="21" t="s">
+      <c r="A220" s="28" t="s">
         <v>929</v>
       </c>
       <c r="C220" s="25" t="s">
@@ -17162,7 +17162,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="221" s="17" spans="1:12">
-      <c r="A221" s="21" t="s">
+      <c r="A221" s="30" t="s">
         <v>932</v>
       </c>
       <c r="C221" s="25" t="s">
@@ -17183,7 +17183,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="222" s="17" spans="1:12">
-      <c r="A222" s="21" t="s">
+      <c r="A222" s="26" t="s">
         <v>936</v>
       </c>
       <c r="C222" s="25" t="n"/>
@@ -17225,7 +17225,7 @@
       </c>
     </row>
     <row customHeight="1" ht="35.95" r="224" s="17" spans="1:12">
-      <c r="A224" s="21" t="s">
+      <c r="A224" s="30" t="s">
         <v>944</v>
       </c>
       <c r="C224" s="25" t="s">
@@ -17250,7 +17250,7 @@
       </c>
     </row>
     <row customHeight="1" ht="46.95" r="225" s="17" spans="1:12">
-      <c r="A225" s="21" t="s">
+      <c r="A225" s="30" t="s">
         <v>950</v>
       </c>
       <c r="C225" s="25" t="n"/>
@@ -17273,7 +17273,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="226" s="17" spans="1:12">
-      <c r="A226" s="21" t="s">
+      <c r="A226" s="26" t="s">
         <v>954</v>
       </c>
       <c r="C226" s="25" t="s">
@@ -17426,7 +17426,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="233" s="17" spans="1:12">
-      <c r="A233" s="21" t="s">
+      <c r="A233" s="26" t="s">
         <v>985</v>
       </c>
       <c r="C233" s="25" t="s">
@@ -17512,7 +17512,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="237" s="17" spans="1:12">
-      <c r="A237" s="21" t="s">
+      <c r="A237" s="28" t="s">
         <v>1002</v>
       </c>
       <c r="C237" s="25" t="s">
@@ -17560,7 +17560,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="239" s="17" spans="1:12">
-      <c r="A239" s="21" t="s">
+      <c r="A239" s="28" t="s">
         <v>1013</v>
       </c>
       <c r="C239" s="25" t="s">
@@ -17650,7 +17650,7 @@
       </c>
     </row>
     <row customHeight="1" ht="35.95" r="243" s="17" spans="1:12">
-      <c r="A243" s="21" t="s">
+      <c r="A243" s="30" t="s">
         <v>1030</v>
       </c>
       <c r="C243" s="22" t="n"/>
@@ -17669,7 +17669,7 @@
       </c>
     </row>
     <row customHeight="1" ht="12.95" r="244" s="17" spans="1:12">
-      <c r="A244" s="21" t="s">
+      <c r="A244" s="30" t="s">
         <v>1033</v>
       </c>
       <c r="C244" s="22" t="n"/>
@@ -17711,7 +17711,7 @@
       </c>
     </row>
     <row customHeight="1" ht="45.95" r="246" s="17" spans="1:12">
-      <c r="A246" s="21" t="s">
+      <c r="A246" s="30" t="s">
         <v>1041</v>
       </c>
       <c r="C246" s="22" t="n"/>
@@ -17734,7 +17734,7 @@
       </c>
     </row>
     <row customHeight="1" ht="35.95" r="247" s="17" spans="1:12">
-      <c r="A247" s="21" t="s">
+      <c r="A247" s="26" t="s">
         <v>1046</v>
       </c>
       <c r="C247" s="22" t="n"/>
@@ -17757,7 +17757,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="248" s="17" spans="1:12">
-      <c r="A248" s="21" t="s">
+      <c r="A248" s="30" t="s">
         <v>1049</v>
       </c>
       <c r="C248" s="25" t="s">
@@ -17836,7 +17836,7 @@
       </c>
     </row>
     <row customHeight="1" ht="34.95" r="251" s="17" spans="1:12">
-      <c r="A251" s="21" t="s">
+      <c r="A251" s="30" t="s">
         <v>1068</v>
       </c>
       <c r="C251" s="22" t="n"/>
@@ -17941,7 +17941,7 @@
       </c>
     </row>
     <row customHeight="1" ht="12.95" r="256" s="17" spans="1:12">
-      <c r="A256" s="21" t="s">
+      <c r="A256" s="26" t="s">
         <v>1088</v>
       </c>
       <c r="C256" s="25" t="n"/>
@@ -17960,7 +17960,7 @@
       </c>
     </row>
     <row customHeight="1" ht="17.95" r="257" s="17" spans="1:12">
-      <c r="A257" s="21" t="s">
+      <c r="A257" s="30" t="s">
         <v>1091</v>
       </c>
       <c r="C257" s="25" t="n"/>
@@ -18021,7 +18021,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="260" s="17" spans="1:12">
-      <c r="A260" s="21" t="s">
+      <c r="A260" s="30" t="s">
         <v>1102</v>
       </c>
       <c r="C260" s="25" t="s">
@@ -18088,7 +18088,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.5" r="263" s="17" spans="1:12">
-      <c r="A263" s="21" t="s">
+      <c r="A263" s="28" t="s">
         <v>1115</v>
       </c>
       <c r="C263" s="21" t="s">
@@ -18147,7 +18147,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="266" s="17" spans="1:12">
-      <c r="A266" s="21" t="s">
+      <c r="A266" s="28" t="s">
         <v>1125</v>
       </c>
       <c r="C266" s="25" t="s">
@@ -18271,7 +18271,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="272" s="17" spans="1:12">
-      <c r="A272" s="26" t="s">
+      <c r="A272" s="30" t="s">
         <v>1148</v>
       </c>
       <c r="C272" s="25" t="n"/>
@@ -18332,7 +18332,7 @@
       </c>
     </row>
     <row customHeight="1" ht="46.95" r="275" s="17" spans="1:12">
-      <c r="A275" s="26" t="s">
+      <c r="A275" s="30" t="s">
         <v>1159</v>
       </c>
       <c r="C275" s="25" t="s">
@@ -18374,7 +18374,7 @@
       </c>
     </row>
     <row customHeight="1" ht="35.95" r="277" s="17" spans="1:12">
-      <c r="A277" s="21" t="s">
+      <c r="A277" s="30" t="s">
         <v>1167</v>
       </c>
       <c r="C277" s="25" t="n"/>
@@ -18416,7 +18416,7 @@
       </c>
     </row>
     <row customHeight="1" ht="12.95" r="279" s="17" spans="1:12">
-      <c r="A279" s="21" t="s">
+      <c r="A279" s="26" t="s">
         <v>1175</v>
       </c>
       <c r="C279" s="25" t="s">
@@ -18435,7 +18435,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="280" s="17" spans="1:12">
-      <c r="A280" s="21" t="s">
+      <c r="A280" s="26" t="s">
         <v>1178</v>
       </c>
       <c r="C280" s="25" t="s">
@@ -18502,7 +18502,7 @@
       </c>
     </row>
     <row customHeight="1" ht="35.95" r="283" s="17" spans="1:12">
-      <c r="A283" s="21" t="s">
+      <c r="A283" s="28" t="s">
         <v>1190</v>
       </c>
       <c r="C283" s="25" t="s">
@@ -18521,7 +18521,7 @@
       </c>
     </row>
     <row customHeight="1" ht="35.95" r="284" s="17" spans="1:12">
-      <c r="A284" s="21" t="s">
+      <c r="A284" s="28" t="s">
         <v>1192</v>
       </c>
       <c r="C284" s="25" t="s">
@@ -18697,7 +18697,7 @@
       </c>
     </row>
     <row customHeight="1" ht="12.95" r="292" s="17" spans="1:12">
-      <c r="A292" s="21" t="s">
+      <c r="A292" s="26" t="s">
         <v>1223</v>
       </c>
       <c r="C292" s="25" t="s">
@@ -18720,7 +18720,7 @@
       </c>
     </row>
     <row customHeight="1" ht="17.95" r="293" s="17" spans="1:12">
-      <c r="A293" s="21" t="s">
+      <c r="A293" s="26" t="s">
         <v>1228</v>
       </c>
       <c r="C293" s="25" t="n"/>
@@ -18739,7 +18739,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="294" s="17" spans="1:12">
-      <c r="A294" s="21" t="s">
+      <c r="A294" s="30" t="s">
         <v>1231</v>
       </c>
       <c r="C294" s="25" t="s">
@@ -18825,7 +18825,7 @@
       </c>
     </row>
     <row customHeight="1" ht="12.95" r="298" s="17" spans="1:12">
-      <c r="A298" s="21" t="s">
+      <c r="A298" s="28" t="s">
         <v>1246</v>
       </c>
       <c r="C298" s="25" t="n"/>
@@ -18844,7 +18844,7 @@
       </c>
     </row>
     <row customHeight="1" ht="35.95" r="299" s="17" spans="1:12">
-      <c r="A299" s="21" t="s">
+      <c r="A299" s="28" t="s">
         <v>1249</v>
       </c>
       <c r="C299" s="25" t="s">
@@ -18867,7 +18867,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="300" s="17" spans="1:12">
-      <c r="A300" s="21" t="s">
+      <c r="A300" s="28" t="s">
         <v>1253</v>
       </c>
       <c r="C300" s="25" t="s">
@@ -18944,7 +18944,7 @@
       </c>
     </row>
     <row customHeight="1" ht="35.95" r="303" s="17" spans="1:12">
-      <c r="A303" s="21" t="s">
+      <c r="A303" s="28" t="s">
         <v>1270</v>
       </c>
       <c r="C303" s="25" t="s">
@@ -18975,7 +18975,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="304" s="17" spans="1:12">
-      <c r="A304" s="21" t="s">
+      <c r="A304" s="28" t="s">
         <v>1279</v>
       </c>
       <c r="C304" s="25" t="n"/>
@@ -19080,7 +19080,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="309" s="17" spans="1:12">
-      <c r="A309" s="21" t="s">
+      <c r="A309" s="28" t="s">
         <v>1299</v>
       </c>
       <c r="C309" s="25" t="n"/>
@@ -19164,7 +19164,7 @@
       </c>
     </row>
     <row customHeight="1" ht="17.95" r="313" s="17" spans="1:12">
-      <c r="A313" s="21" t="s">
+      <c r="A313" s="26" t="s">
         <v>1312</v>
       </c>
       <c r="C313" s="25" t="s">
@@ -19248,7 +19248,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="317" s="17" spans="1:12">
-      <c r="A317" s="21" t="s">
+      <c r="A317" s="30" t="s">
         <v>1328</v>
       </c>
       <c r="C317" s="25" t="n"/>
@@ -19380,7 +19380,7 @@
       </c>
     </row>
     <row customHeight="1" ht="35.95" r="323" s="17" spans="1:12">
-      <c r="A323" s="21" t="s">
+      <c r="A323" s="26" t="s">
         <v>1354</v>
       </c>
       <c r="C323" s="25" t="s">
@@ -19401,7 +19401,7 @@
       </c>
     </row>
     <row customHeight="1" ht="35.95" r="324" s="17" spans="1:12">
-      <c r="A324" s="21" t="s">
+      <c r="A324" s="30" t="s">
         <v>1358</v>
       </c>
       <c r="C324" s="25" t="n"/>
@@ -19447,7 +19447,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="326" s="17" spans="1:12">
-      <c r="A326" s="21" t="s">
+      <c r="A326" s="26" t="s">
         <v>1366</v>
       </c>
       <c r="C326" s="25" t="s">
@@ -19518,7 +19518,7 @@
       </c>
     </row>
     <row customHeight="1" ht="17.95" r="329" s="17" spans="1:12">
-      <c r="A329" s="21" t="s">
+      <c r="A329" s="28" t="s">
         <v>1381</v>
       </c>
       <c r="C329" s="25" t="n"/>
@@ -19556,7 +19556,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="331" s="17" spans="1:12">
-      <c r="A331" s="21" t="s">
+      <c r="A331" s="30" t="s">
         <v>1387</v>
       </c>
       <c r="C331" s="25" t="n"/>
@@ -19684,7 +19684,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="337" s="17" spans="1:12">
-      <c r="A337" s="21" t="s">
+      <c r="A337" s="28" t="s">
         <v>1410</v>
       </c>
       <c r="C337" s="25" t="n"/>
@@ -19766,7 +19766,7 @@
       </c>
     </row>
     <row customHeight="1" ht="35.95" r="341" s="17" spans="1:12">
-      <c r="A341" s="21" t="s">
+      <c r="A341" s="26" t="s">
         <v>1425</v>
       </c>
       <c r="C341" s="25" t="n"/>
@@ -19787,7 +19787,7 @@
       </c>
     </row>
     <row customHeight="1" ht="46.95" r="342" s="17" spans="1:12">
-      <c r="A342" s="30" t="s">
+      <c r="A342" s="28" t="s">
         <v>1429</v>
       </c>
       <c r="C342" s="25" t="n"/>
@@ -19923,7 +19923,7 @@
       </c>
     </row>
     <row customHeight="1" ht="12.95" r="348" s="17" spans="1:12">
-      <c r="A348" s="21" t="s">
+      <c r="A348" s="26" t="s">
         <v>1458</v>
       </c>
       <c r="C348" s="25" t="s">
@@ -19946,7 +19946,7 @@
       </c>
     </row>
     <row customHeight="1" ht="35.95" r="349" s="17" spans="1:12">
-      <c r="A349" s="26" t="s">
+      <c r="A349" s="28" t="s">
         <v>1462</v>
       </c>
       <c r="C349" s="25" t="n"/>
@@ -19965,7 +19965,7 @@
       </c>
     </row>
     <row customHeight="1" ht="35.95" r="350" s="17" spans="1:12">
-      <c r="A350" s="21" t="s">
+      <c r="A350" s="30" t="s">
         <v>1465</v>
       </c>
       <c r="C350" s="25" t="s">
@@ -20051,7 +20051,7 @@
       </c>
     </row>
     <row customHeight="1" ht="12.95" r="354" s="17" spans="1:12">
-      <c r="A354" s="21" t="s">
+      <c r="A354" s="28" t="s">
         <v>1481</v>
       </c>
       <c r="C354" s="25" t="s">
@@ -20070,7 +20070,7 @@
       </c>
     </row>
     <row customHeight="1" ht="46.95" r="355" s="17" spans="1:12">
-      <c r="A355" s="21" t="s">
+      <c r="A355" s="30" t="s">
         <v>1484</v>
       </c>
       <c r="C355" s="25" t="s">
@@ -20108,7 +20108,7 @@
       </c>
     </row>
     <row customHeight="1" ht="35.95" r="357" s="17" spans="1:12">
-      <c r="A357" s="21" t="s">
+      <c r="A357" s="28" t="s">
         <v>1489</v>
       </c>
       <c r="C357" s="25" t="s">
@@ -20175,7 +20175,7 @@
       </c>
     </row>
     <row customHeight="1" ht="46.95" r="360" s="17" spans="1:12">
-      <c r="A360" s="21" t="s">
+      <c r="A360" s="30" t="s">
         <v>1502</v>
       </c>
       <c r="C360" s="25" t="s">
@@ -20221,7 +20221,7 @@
       </c>
     </row>
     <row customHeight="1" ht="35.95" r="362" s="17" spans="1:12">
-      <c r="A362" s="21" t="s">
+      <c r="A362" s="28" t="s">
         <v>1511</v>
       </c>
       <c r="C362" s="25" t="n"/>
@@ -20290,7 +20290,7 @@
       </c>
     </row>
     <row customHeight="1" ht="46.95" r="365" s="17" spans="1:12">
-      <c r="A365" s="21" t="s">
+      <c r="A365" s="30" t="s">
         <v>1525</v>
       </c>
       <c r="C365" s="25" t="s">
@@ -20380,7 +20380,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="369" s="17" spans="1:12">
-      <c r="A369" s="21" t="s">
+      <c r="A369" s="30" t="s">
         <v>1541</v>
       </c>
       <c r="C369" s="25" t="s">
@@ -20451,7 +20451,7 @@
       </c>
     </row>
     <row customHeight="1" ht="17.95" r="372" s="17" spans="1:12">
-      <c r="A372" s="26" t="s">
+      <c r="A372" s="28" t="s">
         <v>1555</v>
       </c>
       <c r="C372" s="25" t="n"/>
@@ -20493,7 +20493,7 @@
       </c>
     </row>
     <row customHeight="1" ht="35.95" r="374" s="17" spans="1:12">
-      <c r="A374" s="21" t="s">
+      <c r="A374" s="28" t="s">
         <v>1563</v>
       </c>
       <c r="C374" s="25" t="s">
@@ -20575,7 +20575,7 @@
       </c>
     </row>
     <row customHeight="1" ht="17.95" r="378" s="17" spans="1:12">
-      <c r="A378" s="21" t="s">
+      <c r="A378" s="30" t="s">
         <v>1578</v>
       </c>
       <c r="C378" s="25" t="s">
@@ -20619,7 +20619,7 @@
       </c>
     </row>
     <row customHeight="1" ht="46.95" r="380" s="17" spans="1:12">
-      <c r="A380" s="21" t="s">
+      <c r="A380" s="26" t="s">
         <v>1587</v>
       </c>
       <c r="C380" s="25" t="n"/>
@@ -20638,7 +20638,7 @@
       </c>
     </row>
     <row customHeight="1" ht="35.95" r="381" s="17" spans="1:12">
-      <c r="A381" s="21" t="s">
+      <c r="A381" s="28" t="s">
         <v>1590</v>
       </c>
       <c r="C381" s="25" t="n"/>
@@ -20657,7 +20657,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="382" s="17" spans="1:12">
-      <c r="A382" s="21" t="s">
+      <c r="A382" s="28" t="s">
         <v>1593</v>
       </c>
       <c r="C382" s="25" t="s">
@@ -20728,7 +20728,7 @@
       </c>
     </row>
     <row customHeight="1" ht="23.7" r="385" s="17" spans="1:12">
-      <c r="A385" s="21" t="s">
+      <c r="A385" s="28" t="s">
         <v>1605</v>
       </c>
       <c r="C385" s="25" t="s">
@@ -20891,7 +20891,7 @@
       </c>
     </row>
     <row customHeight="1" ht="35.95" r="392" s="17" spans="1:12">
-      <c r="A392" s="21" t="s">
+      <c r="A392" s="28" t="s">
         <v>1638</v>
       </c>
       <c r="C392" s="25" t="s">
@@ -20941,7 +20941,7 @@
       </c>
     </row>
     <row customHeight="1" ht="17.95" r="394" s="17" spans="1:12">
-      <c r="A394" s="21" t="s">
+      <c r="A394" s="28" t="s">
         <v>1650</v>
       </c>
       <c r="C394" s="25" t="s">
@@ -21002,7 +21002,7 @@
       </c>
     </row>
     <row customHeight="1" ht="12.95" r="397" s="17" spans="1:12">
-      <c r="A397" s="21" t="s">
+      <c r="A397" s="28" t="s">
         <v>1661</v>
       </c>
       <c r="C397" s="25" t="n"/>
@@ -21065,7 +21065,7 @@
       </c>
     </row>
     <row customHeight="1" ht="46.95" r="400" s="17" spans="1:12">
-      <c r="A400" s="21" t="s">
+      <c r="A400" s="28" t="s">
         <v>1672</v>
       </c>
       <c r="C400" s="25" t="n"/>
@@ -21084,7 +21084,7 @@
       </c>
     </row>
     <row customHeight="1" ht="46.95" r="401" s="17" spans="1:12">
-      <c r="A401" s="21" t="s">
+      <c r="A401" s="30" t="s">
         <v>1675</v>
       </c>
       <c r="C401" s="25" t="s">
@@ -21107,7 +21107,7 @@
       </c>
     </row>
     <row customHeight="1" ht="35.95" r="402" s="17" spans="1:12">
-      <c r="A402" s="21" t="s">
+      <c r="A402" s="28" t="s">
         <v>1679</v>
       </c>
       <c r="C402" s="25" t="s">
@@ -21256,7 +21256,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="409" s="17" spans="1:12">
-      <c r="A409" s="21" t="s">
+      <c r="A409" s="26" t="s">
         <v>1703</v>
       </c>
       <c r="C409" s="25" t="n"/>
@@ -21298,7 +21298,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="411" s="17" spans="1:12">
-      <c r="A411" s="21" t="s">
+      <c r="A411" s="26" t="s">
         <v>1710</v>
       </c>
       <c r="C411" s="25" t="n"/>
@@ -21317,7 +21317,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="412" s="17" spans="1:12">
-      <c r="A412" s="21" t="s">
+      <c r="A412" s="30" t="s">
         <v>1713</v>
       </c>
       <c r="C412" s="25" t="s">
@@ -21340,7 +21340,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="413" s="17" spans="1:12">
-      <c r="A413" s="21" t="s">
+      <c r="A413" s="28" t="s">
         <v>1717</v>
       </c>
       <c r="C413" s="25" t="n"/>
@@ -21386,7 +21386,7 @@
       </c>
     </row>
     <row customHeight="1" ht="35.95" r="415" s="17" spans="1:12">
-      <c r="A415" s="21" t="s">
+      <c r="A415" s="30" t="s">
         <v>1726</v>
       </c>
       <c r="C415" s="25" t="s">
@@ -21557,7 +21557,7 @@
       </c>
     </row>
     <row customHeight="1" ht="17.95" r="422" s="17" spans="1:12">
-      <c r="A422" s="21" t="s">
+      <c r="A422" s="30" t="s">
         <v>1766</v>
       </c>
       <c r="C422" s="25" t="n"/>
@@ -21576,7 +21576,7 @@
       </c>
     </row>
     <row customHeight="1" ht="35.95" r="423" s="17" spans="1:12">
-      <c r="A423" s="21" t="s">
+      <c r="A423" s="28" t="s">
         <v>1769</v>
       </c>
       <c r="C423" s="25" t="s">
@@ -21710,7 +21710,7 @@
       </c>
     </row>
     <row customHeight="1" ht="58.45" r="429" s="17" spans="1:12">
-      <c r="A429" s="30" t="s">
+      <c r="A429" s="28" t="s">
         <v>1794</v>
       </c>
       <c r="C429" s="25" t="n"/>
@@ -21733,7 +21733,7 @@
       </c>
     </row>
     <row customHeight="1" ht="46.95" r="430" s="17" spans="1:12">
-      <c r="A430" s="21" t="s">
+      <c r="A430" s="30" t="s">
         <v>1799</v>
       </c>
       <c r="C430" s="25" t="n"/>
@@ -21754,7 +21754,7 @@
       </c>
     </row>
     <row customHeight="1" ht="12.95" r="431" s="17" spans="1:12">
-      <c r="A431" s="21" t="s">
+      <c r="A431" s="28" t="s">
         <v>1802</v>
       </c>
       <c r="C431" s="25" t="s">
@@ -21850,7 +21850,7 @@
       </c>
     </row>
     <row customHeight="1" ht="46.95" r="435" s="17" spans="1:12">
-      <c r="A435" s="26" t="s">
+      <c r="A435" s="28" t="s">
         <v>1824</v>
       </c>
       <c r="C435" s="25" t="s">
@@ -21913,7 +21913,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="438" s="17" spans="1:12">
-      <c r="A438" s="21" t="s">
+      <c r="A438" s="30" t="s">
         <v>1835</v>
       </c>
       <c r="C438" s="25" t="s">
@@ -21936,7 +21936,7 @@
       </c>
     </row>
     <row customHeight="1" ht="17.95" r="439" s="17" spans="1:12">
-      <c r="A439" s="21" t="s">
+      <c r="A439" s="30" t="s">
         <v>1840</v>
       </c>
       <c r="C439" s="25" t="s">
@@ -22111,7 +22111,7 @@
       </c>
     </row>
     <row customHeight="1" ht="35.95" r="446" s="17" spans="1:12">
-      <c r="A446" s="21" t="s">
+      <c r="A446" s="30" t="s">
         <v>1878</v>
       </c>
       <c r="C446" s="25" t="s">
@@ -22165,7 +22165,7 @@
       </c>
     </row>
     <row customHeight="1" ht="45.95" r="448" s="17" spans="1:12">
-      <c r="A448" s="21" t="s">
+      <c r="A448" s="28" t="s">
         <v>1892</v>
       </c>
       <c r="C448" s="25" t="n"/>
@@ -22205,7 +22205,7 @@
       </c>
     </row>
     <row customHeight="1" ht="58.45" r="450" s="17" spans="1:12">
-      <c r="A450" s="21" t="s">
+      <c r="A450" s="26" t="s">
         <v>1899</v>
       </c>
       <c r="C450" s="25" t="n"/>
@@ -22243,7 +22243,7 @@
       </c>
     </row>
     <row customHeight="1" ht="58.45" r="452" s="17" spans="1:12">
-      <c r="A452" s="21" t="s">
+      <c r="A452" s="30" t="s">
         <v>1904</v>
       </c>
       <c r="C452" s="25" t="n"/>
@@ -22354,7 +22354,7 @@
       </c>
     </row>
     <row customHeight="1" ht="35.95" r="457" s="17" spans="1:12">
-      <c r="A457" s="21" t="s">
+      <c r="A457" s="28" t="s">
         <v>1924</v>
       </c>
       <c r="C457" s="25" t="s">
@@ -22380,7 +22380,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="458" s="17" spans="1:12">
-      <c r="A458" s="21" t="s">
+      <c r="A458" s="30" t="s">
         <v>1931</v>
       </c>
       <c r="C458" s="25" t="s">
@@ -22550,7 +22550,7 @@
       </c>
     </row>
     <row customHeight="1" ht="35.95" r="466" s="17" spans="1:12">
-      <c r="A466" s="21" t="s">
+      <c r="A466" s="26" t="s">
         <v>1965</v>
       </c>
       <c r="C466" s="25" t="s">
@@ -22690,7 +22690,7 @@
       </c>
     </row>
     <row customHeight="1" ht="78.95" r="472" s="17" spans="1:12">
-      <c r="A472" s="21" t="s">
+      <c r="A472" s="30" t="s">
         <v>1998</v>
       </c>
       <c r="C472" s="25" t="n"/>
@@ -22732,7 +22732,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="474" s="17" spans="1:12">
-      <c r="A474" s="21" t="s">
+      <c r="A474" s="30" t="s">
         <v>2005</v>
       </c>
       <c r="C474" s="25" t="s">
@@ -22750,7 +22750,7 @@
       </c>
     </row>
     <row customHeight="1" ht="58.45" r="475" s="17" spans="1:12">
-      <c r="A475" s="21" t="s">
+      <c r="A475" s="28" t="s">
         <v>2008</v>
       </c>
       <c r="C475" s="25" t="s">
@@ -22870,7 +22870,7 @@
       </c>
     </row>
     <row customHeight="1" ht="35.95" r="480" s="17" spans="1:12">
-      <c r="A480" s="21" t="s">
+      <c r="A480" s="28" t="s">
         <v>2037</v>
       </c>
       <c r="C480" s="25" t="s">
@@ -22888,7 +22888,7 @@
       </c>
     </row>
     <row customHeight="1" ht="35.95" r="481" s="17" spans="1:12">
-      <c r="A481" s="21" t="s">
+      <c r="A481" s="28" t="s">
         <v>2040</v>
       </c>
       <c r="C481" s="25" t="n"/>
@@ -22934,7 +22934,7 @@
       </c>
     </row>
     <row customHeight="1" ht="35.95" r="483" s="17" spans="1:12">
-      <c r="A483" s="21" t="s">
+      <c r="A483" s="30" t="s">
         <v>2050</v>
       </c>
       <c r="C483" s="25" t="s">
@@ -22978,7 +22978,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="485" s="17" spans="1:12">
-      <c r="A485" s="21" t="s">
+      <c r="A485" s="30" t="s">
         <v>2060</v>
       </c>
       <c r="C485" s="25" t="s">
@@ -23060,7 +23060,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="489" s="17" spans="1:12">
-      <c r="A489" s="21" t="s">
+      <c r="A489" s="26" t="s">
         <v>2077</v>
       </c>
       <c r="C489" s="25" t="s">
@@ -23082,7 +23082,7 @@
       </c>
     </row>
     <row customHeight="1" ht="12.8" r="490" s="17" spans="1:12">
-      <c r="A490" s="21" t="s">
+      <c r="A490" s="30" t="s">
         <v>2082</v>
       </c>
       <c r="C490" s="25" t="s">
@@ -23136,7 +23136,7 @@
       </c>
     </row>
     <row customHeight="1" ht="12.8" r="493" s="17" spans="1:12">
-      <c r="A493" s="21" t="s">
+      <c r="A493" s="26" t="s">
         <v>2091</v>
       </c>
       <c r="C493" s="25" t="n"/>
@@ -23154,7 +23154,7 @@
       </c>
     </row>
     <row customHeight="1" ht="24.45" r="494" s="17" spans="1:12">
-      <c r="A494" s="30" t="s">
+      <c r="A494" s="28" t="s">
         <v>2094</v>
       </c>
       <c r="C494" s="25" t="n"/>
@@ -23188,7 +23188,7 @@
       <c r="L495" s="29" t="n"/>
     </row>
     <row customHeight="1" ht="12.8" r="496" s="17" spans="1:12">
-      <c r="A496" s="21" t="s">
+      <c r="A496" s="30" t="s">
         <v>2099</v>
       </c>
       <c r="C496" s="25" t="n"/>
@@ -23210,7 +23210,7 @@
       </c>
     </row>
     <row customHeight="1" ht="12.8" r="497" s="17" spans="1:12">
-      <c r="A497" s="21" t="s">
+      <c r="A497" s="26" t="s">
         <v>2104</v>
       </c>
       <c r="C497" s="25" t="s">
@@ -23256,7 +23256,7 @@
       </c>
     </row>
     <row customHeight="1" ht="12.8" r="499" s="17" spans="1:12">
-      <c r="A499" s="21" t="s">
+      <c r="A499" s="30" t="s">
         <v>2115</v>
       </c>
       <c r="C499" s="25" t="n"/>
@@ -23274,7 +23274,7 @@
       </c>
     </row>
     <row customHeight="1" ht="12.8" r="500" s="17" spans="1:12">
-      <c r="A500" s="30" t="s">
+      <c r="A500" s="28" t="s">
         <v>2118</v>
       </c>
       <c r="C500" s="25" t="s">
@@ -23302,7 +23302,7 @@
       </c>
     </row>
     <row customHeight="1" ht="12.8" r="501" s="17" spans="1:12">
-      <c r="A501" s="21" t="s">
+      <c r="A501" s="28" t="s">
         <v>2125</v>
       </c>
       <c r="C501" s="25" t="s">
@@ -23402,7 +23402,7 @@
       </c>
     </row>
     <row customHeight="1" ht="17.95" r="506" s="17" spans="1:12">
-      <c r="A506" s="21" t="s">
+      <c r="A506" s="28" t="s">
         <v>2147</v>
       </c>
       <c r="C506" s="25" t="n"/>
@@ -23417,7 +23417,7 @@
       <c r="L506" s="29" t="n"/>
     </row>
     <row customHeight="1" ht="23.85" r="507" s="17" spans="1:12">
-      <c r="A507" s="21" t="s">
+      <c r="A507" s="30" t="s">
         <v>2149</v>
       </c>
       <c r="C507" s="25" t="s">
@@ -23512,7 +23512,7 @@
       </c>
     </row>
     <row customHeight="1" ht="23.85" r="512" s="17" spans="1:12">
-      <c r="A512" s="21" t="s">
+      <c r="A512" s="26" t="s">
         <v>2169</v>
       </c>
       <c r="C512" s="25" t="n"/>
@@ -23618,7 +23618,7 @@
       </c>
     </row>
     <row customHeight="1" ht="35.95" r="518" s="17" spans="1:12">
-      <c r="A518" s="21" t="s">
+      <c r="A518" s="30" t="s">
         <v>2187</v>
       </c>
       <c r="C518" s="25" t="s">
@@ -23637,7 +23637,7 @@
       </c>
     </row>
     <row customHeight="1" ht="58.45" r="519" s="17" spans="1:12">
-      <c r="A519" s="21" t="s">
+      <c r="A519" s="30" t="s">
         <v>2191</v>
       </c>
       <c r="C519" s="25" t="s">
@@ -23755,7 +23755,7 @@
       </c>
     </row>
     <row customHeight="1" ht="23.85" r="525" s="17" spans="1:12">
-      <c r="A525" s="21" t="s">
+      <c r="A525" s="26" t="s">
         <v>2214</v>
       </c>
       <c r="C525" s="25" t="s">
@@ -23862,7 +23862,7 @@
       </c>
     </row>
     <row customHeight="1" ht="57.45" r="530" s="17" spans="1:12">
-      <c r="A530" s="21" t="s">
+      <c r="A530" s="26" t="s">
         <v>2237</v>
       </c>
       <c r="C530" s="25" t="s">
@@ -24016,7 +24016,7 @@
       </c>
     </row>
     <row customHeight="1" ht="57.45" r="538" s="17" spans="1:12">
-      <c r="A538" s="21" t="s">
+      <c r="A538" s="30" t="s">
         <v>2267</v>
       </c>
       <c r="C538" s="25" t="n"/>
@@ -24084,7 +24084,7 @@
       </c>
     </row>
     <row customHeight="1" ht="17.15" r="542" s="17" spans="1:12">
-      <c r="A542" s="21" t="s">
+      <c r="A542" s="28" t="s">
         <v>2277</v>
       </c>
       <c r="C542" s="25" t="n"/>
@@ -24143,7 +24143,7 @@
       </c>
     </row>
     <row customHeight="1" ht="68.65000000000001" r="545" s="17" spans="1:12">
-      <c r="A545" s="21" t="s">
+      <c r="A545" s="30" t="s">
         <v>2289</v>
       </c>
       <c r="C545" s="25" t="s">
@@ -24181,7 +24181,7 @@
       </c>
     </row>
     <row customHeight="1" ht="23.85" r="547" s="17" spans="1:12">
-      <c r="A547" s="21" t="s">
+      <c r="A547" s="28" t="s">
         <v>2298</v>
       </c>
       <c r="C547" s="25" t="s">

</xml_diff>